<commit_message>
Changes in ExcelParseTest and Excel files
</commit_message>
<xml_diff>
--- a/src/test/resources/test6.xlsx
+++ b/src/test/resources/test6.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17625" windowHeight="7065"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14835" windowHeight="5865"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -26,51 +26,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Nombre</t>
   </si>
   <si>
-    <t>C/ Federico García Lorca 2</t>
-  </si>
-  <si>
-    <t>Apellidos</t>
-  </si>
-  <si>
-    <t>Juan</t>
-  </si>
-  <si>
-    <t>Torres Pardo</t>
-  </si>
-  <si>
-    <t>DNI</t>
-  </si>
-  <si>
-    <t>Fecha nacimiento</t>
-  </si>
-  <si>
-    <t>Nacionalidad</t>
-  </si>
-  <si>
-    <t>Español</t>
-  </si>
-  <si>
     <t>Correo electrónico</t>
   </si>
   <si>
     <t>juan@example.com</t>
   </si>
   <si>
-    <t>Dirección postal</t>
-  </si>
-  <si>
-    <t>NIF</t>
-  </si>
-  <si>
-    <t>pollingStation</t>
-  </si>
-  <si>
-    <t>90500084Y</t>
+    <t>Localización</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>Juan Torres Pardo</t>
+  </si>
+  <si>
+    <t>40.5N30.99W</t>
+  </si>
+  <si>
+    <t>58758L</t>
   </si>
 </sst>
 </file>
@@ -115,9 +97,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -403,7 +384,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -413,60 +394,35 @@
     <col min="5" max="5" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="D2" t="s">
         <v>8</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>